<commit_message>
fixed compute horizontal score algorithm
</commit_message>
<xml_diff>
--- a/src/main/java/com/catapult/excel/analyzer/ui/test1.xlsx
+++ b/src/main/java/com/catapult/excel/analyzer/ui/test1.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
   <si>
     <t>HEADER1</t>
   </si>
@@ -57,16 +57,25 @@
     <t>SH1</t>
   </si>
   <si>
-    <t>SH2</t>
-  </si>
-  <si>
     <t>SH3</t>
   </si>
   <si>
-    <t>SH4</t>
-  </si>
-  <si>
     <t>SH5</t>
+  </si>
+  <si>
+    <t>SH21</t>
+  </si>
+  <si>
+    <t>SH22</t>
+  </si>
+  <si>
+    <t>SH23</t>
+  </si>
+  <si>
+    <t>SH24</t>
+  </si>
+  <si>
+    <t>SH25</t>
   </si>
 </sst>
 </file>
@@ -104,7 +113,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -112,13 +121,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,55 +445,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F8"/>
+  <dimension ref="B2:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -505,10 +528,21 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="F8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -522,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed compute horizontal score algorithm and processing of subheaders
</commit_message>
<xml_diff>
--- a/src/main/java/com/catapult/excel/analyzer/ui/test1.xlsx
+++ b/src/main/java/com/catapult/excel/analyzer/ui/test1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
   <si>
     <t>HEADER1</t>
   </si>
@@ -57,9 +57,6 @@
     <t>SH1</t>
   </si>
   <si>
-    <t>SH3</t>
-  </si>
-  <si>
     <t>SH5</t>
   </si>
   <si>
@@ -76,6 +73,12 @@
   </si>
   <si>
     <t>SH25</t>
+  </si>
+  <si>
+    <t>SH4</t>
+  </si>
+  <si>
+    <t>SH2</t>
   </si>
 </sst>
 </file>
@@ -448,7 +451,7 @@
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,30 +471,32 @@
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>